<commit_message>
xlsx properly holds multiple entries with no index
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,20 +458,42 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Vincent Huang</t>
+          <t>Adam Jackson</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Licensed Administrator</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Vancouver, BC</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>RE/MAX Select Properties</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Sarka Trileta</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>Sales Representative</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Vancouver, BC</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>RE/MAX City Realty</t>
         </is>

</xml_diff>

<commit_message>
Checks name in master file for duplicates
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,7 +458,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Cecil Lee</t>
+          <t>David Malkin</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -473,19 +473,19 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>RE/MAX City Realty</t>
+          <t>RE/MAX Select Properties</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ryan Taylor</t>
+          <t>Shahina Najmidinova</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Sales Representative</t>
+          <t>Licensed Administrator</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -495,14 +495,14 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>RE/MAX Real Estate Services</t>
+          <t>RE/MAX City Realty</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Rene Pantoja</t>
+          <t>Leanne Yan</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -517,19 +517,19 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>RE/MAX Crest Realty (South Granville)</t>
+          <t>RE/MAX Real Estate Services</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Valentino Cernica</t>
+          <t>Nicola Campbell</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Realtor</t>
+          <t>Sales Representative</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,19 +539,19 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>RE/MAX Select Properties</t>
+          <t>RE/MAX Crest Realty (South Granville)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Teresa Chan</t>
+          <t>Hazem Sultan</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Sales Representative</t>
+          <t>Real Estate Advisor</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -561,14 +561,14 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>RE/MAX City Realty</t>
+          <t>RE/MAX Crest Realty (South Granville)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Andrew Hasman</t>
+          <t>Meet Dusange</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -583,19 +583,19 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>RE/MAX Real Estate Services</t>
+          <t>RE/MAX City Realty</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Michael Pearlman</t>
+          <t>Khush Grewal</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sales Representative</t>
+          <t>Realtor</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -605,19 +605,19 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>RE/MAX Select Properties</t>
+          <t>RE/MAX Elevate</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mehrnoush Hemmati-Asl</t>
+          <t>Gabe Bandel</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Sales associate.</t>
+          <t>Licensed Administrator</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -627,19 +627,19 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>RE/MAX City Realty</t>
+          <t>RE/MAX Select Realty</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Bharti Jain</t>
+          <t>James L Wang</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Real Estate Associate</t>
+          <t>Sales Representative</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -656,7 +656,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Aloke Chowdhury</t>
+          <t>Lina Rached</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -671,19 +671,19 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>RE/MAX City Realty</t>
+          <t>RE/MAX Crest Realty (South Granville)</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Ian Malkin</t>
+          <t>Rosalee McRae</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sales Representative</t>
+          <t>Broker</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -693,29 +693,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>RE/MAX Select Realty</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Jan Chan</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Sales Representative</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Vancouver, BC</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>RE/MAX Crest Realty (South Granville)</t>
+          <t>RE/MAX Select Properties</t>
         </is>
       </c>
     </row>

</xml_diff>